<commit_message>
Update AI system - Refactor
</commit_message>
<xml_diff>
--- a/FakeXCOM/Content/Annexes/AlienAI_UM.xlsx
+++ b/FakeXCOM/Content/Annexes/AlienAI_UM.xlsx
@@ -175,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +194,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,10 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +515,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,10 +562,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -621,10 +628,10 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -658,10 +665,10 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update AI system - Debug score on target
</commit_message>
<xml_diff>
--- a/FakeXCOM/Content/Annexes/AlienAI_UM.xlsx
+++ b/FakeXCOM/Content/Annexes/AlienAI_UM.xlsx
@@ -196,7 +196,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,7 +515,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" activeCellId="5" sqref="A20 B20 B15 A15 A6 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update AI - Curve value example
</commit_message>
<xml_diff>
--- a/FakeXCOM/Content/Annexes/AlienAI_UM.xlsx
+++ b/FakeXCOM/Content/Annexes/AlienAI_UM.xlsx
@@ -201,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,15 +209,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +526,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" activeCellId="5" sqref="A20 B20 B15 A15 A6 B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -626,12 +637,13 @@
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -657,18 +669,18 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>